<commit_message>
update SSR and TR
</commit_message>
<xml_diff>
--- a/SSR/SSR_v1.0.xlsx
+++ b/SSR/SSR_v1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bo/Documents/projects/DomainModelExtractor/SSR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0BD7E6-122C-0445-8E3E-CD84DCAFCE3E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40AF7AFD-897A-0B48-8218-BBFF22968072}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="460" windowWidth="22140" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12260" yWindow="2000" windowWidth="19540" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="update_SSR" sheetId="1" r:id="rId1"/>
@@ -1068,7 +1068,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1246,6 +1246,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1409,11 +1415,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1771,14 +1779,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="55.6640625" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1900,20 +1908,20 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1934,51 +1942,51 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2108,17 +2116,17 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="3" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>